<commit_message>
Coding up Final, CPU design
</commit_message>
<xml_diff>
--- a/lab12/IO_Pad.xlsx
+++ b/lab12/IO_Pad.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacky\Desktop\ic_lab_2023\IC_LAB_2023\lab12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B2398C-BD03-4FCB-A928-E306643F329A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F256CA23-86A0-493A-995B-24BF68BE13EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <definedName name="PAD">工作表1!$J$23:$W$36</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>Input</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -364,6 +365,9 @@
   </si>
   <si>
     <t>I_MATRIX_IDX3</t>
+  </si>
+  <si>
+    <t>因ㄨㄟ</t>
   </si>
 </sst>
 </file>
@@ -1037,6 +1041,9 @@
       </c>
       <c r="V23" s="15"/>
       <c r="W23" s="15"/>
+      <c r="AC23" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="24" spans="1:37">
       <c r="A24" s="5"/>

</xml_diff>